<commit_message>
Add test data. Add Motor mount
</commit_message>
<xml_diff>
--- a/Testbenches/HCSR04_result_021119/result_table.xlsx
+++ b/Testbenches/HCSR04_result_021119/result_table.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weil\Documents\Repos\IEEESoutheastCon2019\Testbenches\HCSR04_result_021119\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2D77BF5E-89B4-4AA6-8645-A4D3778CAD90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40D5BEAB-CA53-4C76-A15F-CEC700259BA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="10800"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="10800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_50mm" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="4">
   <si>
     <t>Real(mm)</t>
   </si>
@@ -37,7 +44,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -596,7 +603,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -609,8 +616,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="2400" b="1"/>
-              <a:t>HC-SR04 Measurements</a:t>
+              <a:rPr lang="en-US" sz="4000" b="0"/>
+              <a:t>HC-SR04 Test Results</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -628,7 +635,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -6150,7 +6157,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -6163,14 +6170,14 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:rPr lang="en-US" sz="2400" b="1"/>
                   <a:t>Actual</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
+                  <a:rPr lang="en-US" sz="2400" b="1" baseline="0"/>
                   <a:t> Distance (mm)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1400" b="1"/>
+                <a:endParaRPr lang="en-US" sz="2400" b="1"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -6187,7 +6194,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -6225,7 +6232,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6243,7 +6250,8 @@
         <c:crossAx val="1909422496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="50"/>
+        <c:majorUnit val="100"/>
+        <c:minorUnit val="50"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1909422496"/>
@@ -6273,7 +6281,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -6286,7 +6294,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400" b="1"/>
+                  <a:rPr lang="en-US" sz="2400" b="1"/>
                   <a:t>Measured Distance (mm)</a:t>
                 </a:r>
               </a:p>
@@ -6305,7 +6313,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -6343,7 +6351,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -6361,7 +6369,8 @@
         <c:crossAx val="1912704560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="50"/>
+        <c:majorUnit val="100"/>
+        <c:minorUnit val="50"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -7301,11 +7310,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D901"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A374" workbookViewId="0">
-      <selection activeCell="C91" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>